<commit_message>
Removing useless folder path
</commit_message>
<xml_diff>
--- a/private.xlsx
+++ b/private.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paula/Desktop/Programowanie/Wysylanie_meila/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BE0B71-B041-DD4C-8415-93E28471A23B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99366AE4-C72E-CB49-8F5F-6E1ACB30DB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="26020" windowHeight="15840" xr2:uid="{DBAF6581-D885-C94E-9BBC-3ACA15071CB9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>variable</t>
   </si>
@@ -39,9 +39,6 @@
     <t>private name</t>
   </si>
   <si>
-    <t>*PATH_TO_PICTURES*</t>
-  </si>
-  <si>
     <t>*PATH_TO_DANE.TXT*</t>
   </si>
   <si>
@@ -64,6 +61,30 @@
   </si>
   <si>
     <t>*PATH_TO_ATTACHMENTS_DIR*</t>
+  </si>
+  <si>
+    <t>absolute path to directory where attachments will be saved</t>
+  </si>
+  <si>
+    <t>sender's email address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sender's host </t>
+  </si>
+  <si>
+    <t>sender's password for his email address</t>
+  </si>
+  <si>
+    <t>absolute path to directory where attachments will be archived</t>
+  </si>
+  <si>
+    <t>absolute path to file with data that will be opened in this notepad</t>
+  </si>
+  <si>
+    <t>absolute path to empty file 'export.csv'</t>
+  </si>
+  <si>
+    <t>receiver's email adddress</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -134,18 +155,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -462,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B9B972-BA83-5146-BF09-895DDC6B091E}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -474,7 +524,7 @@
     <col min="2" max="2" width="57.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -482,61 +532,87 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="B10" s="1"/>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Mock files added to be able to run app
</commit_message>
<xml_diff>
--- a/private.xlsx
+++ b/private.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Paula/Desktop/Programowanie/Wysylanie_meila/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99366AE4-C72E-CB49-8F5F-6E1ACB30DB02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341AD5D5-214A-2B44-811A-61A75E1E203D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="460" windowWidth="26020" windowHeight="15840" xr2:uid="{DBAF6581-D885-C94E-9BBC-3ACA15071CB9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>variable</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>receiver's email adddress</t>
+  </si>
+  <si>
+    <t>data.txt</t>
+  </si>
+  <si>
+    <t>export.csv</t>
   </si>
 </sst>
 </file>
@@ -515,7 +521,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,7 +591,9 @@
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -594,7 +602,9 @@
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C9" t="s">
         <v>16</v>
       </c>

</xml_diff>